<commit_message>
Added a time check for master logout only times between 4 pm and 10pm
</commit_message>
<xml_diff>
--- a/room schedule.xlsx
+++ b/room schedule.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
   </bookViews>
@@ -695,7 +690,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -737,9 +732,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -788,7 +780,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -821,26 +813,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -873,23 +848,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1068,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D882"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A856" workbookViewId="0">
-      <selection activeCell="A881" sqref="A881:C881"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13278,10 +13236,10 @@
         <v>221</v>
       </c>
       <c r="B874" s="1">
-        <v>0.75</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C874" s="1">
-        <v>0.875</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D874" t="s">
         <v>7</v>
@@ -13290,6 +13248,12 @@
     <row r="875" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A875" t="s">
         <v>9</v>
+      </c>
+      <c r="B875" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C875" s="1">
+        <v>0.875</v>
       </c>
       <c r="D875" t="s">
         <v>7</v>
@@ -13370,10 +13334,10 @@
         <v>222</v>
       </c>
       <c r="B881" s="1">
-        <v>0.75</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C881" s="1">
-        <v>0.875</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D881" t="s">
         <v>7</v>
@@ -13382,6 +13346,12 @@
     <row r="882" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A882" t="s">
         <v>9</v>
+      </c>
+      <c r="B882" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C882" s="1">
+        <v>0.875</v>
       </c>
       <c r="D882" t="s">
         <v>7</v>

</xml_diff>